<commit_message>
Completed section 2.3.1, distributing the BEA's breakdown of fixed assets across industry and sector.  The script now calculates FA economic depreciation rates for industry and sector using BEA data on depreciation rates by asset type.
</commit_message>
<xml_diff>
--- a/Data/Calibration/DepreciationParameters/Program/data/SOI_Partner/Crosswalks/12pa05_Crosswalk.xlsx
+++ b/Data/Calibration/DepreciationParameters/Program/data/SOI_Partner/Crosswalks/12pa05_Crosswalk.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>All industries</t>
   </si>
@@ -129,6 +129,48 @@
   </si>
   <si>
     <t>53111</t>
+  </si>
+  <si>
+    <t>Securities and commodity contracts and exchanges</t>
+  </si>
+  <si>
+    <t>5231.5232</t>
+  </si>
+  <si>
+    <t>Other finance and insurance</t>
+  </si>
+  <si>
+    <t>521.522.524</t>
+  </si>
+  <si>
+    <t>Real estate</t>
+  </si>
+  <si>
+    <t>531</t>
+  </si>
+  <si>
+    <t>Lessors of nonresidential buildings (except mini-warehouses)</t>
+  </si>
+  <si>
+    <t>lessors of miniwarehouses and self-storage units</t>
+  </si>
+  <si>
+    <t>lessors of other real estate activities</t>
+  </si>
+  <si>
+    <t>53112</t>
+  </si>
+  <si>
+    <t>53113</t>
+  </si>
+  <si>
+    <t>53119</t>
+  </si>
+  <si>
+    <t>5312.5313</t>
+  </si>
+  <si>
+    <t>Nature of business not allocable</t>
   </si>
 </sst>
 </file>
@@ -463,11 +505,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -580,114 +620,167 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
-        <v>5239</v>
+        <v>35</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4">
-        <v>525</v>
+        <v>5239</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>13</v>
+      </c>
+      <c r="B16" s="4">
+        <v>525</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4">
-        <v>53139</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4">
-        <v>54</v>
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4">
-        <v>55</v>
+        <v>41</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="4">
-        <v>56</v>
+        <v>42</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="4">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="4">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4">
-        <v>71</v>
+        <v>17</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B26" s="4">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B33" s="4">
         <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>